<commit_message>
Update Plan de Pruebas Ejercici practico LATAM.xlsx
</commit_message>
<xml_diff>
--- a/Plan de Pruebas Ejercici practico LATAM.xlsx
+++ b/Plan de Pruebas Ejercici practico LATAM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Plan de Pruebas" sheetId="1" r:id="rId1"/>
@@ -1475,6 +1475,186 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1485,27 +1665,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1529,166 +1688,10 @@
     <xf numFmtId="0" fontId="17" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1699,9 +1702,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1742,7 +1742,7 @@
         <xdr:cNvPr id="7" name="1 Grupo">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1761,7 +1761,7 @@
           <xdr:cNvPr id="8" name="2 Triángulo isósceles">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1805,7 +1805,7 @@
           <xdr:cNvPr id="9" name="3 CuadroTexto">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000009000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1857,7 +1857,7 @@
           <xdr:cNvPr id="10" name="4 CuadroTexto">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000A000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1908,7 +1908,7 @@
           <xdr:cNvPr id="11" name="5 CuadroTexto">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000B000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1977,7 +1977,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2040,7 +2040,7 @@
         <xdr:cNvPr id="13" name="Flecha: a la derecha 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C8F414B-1B05-424D-AEBD-0397129D474E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2C8F414B-1B05-424D-AEBD-0397129D474E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2111,7 +2111,7 @@
         <xdr:cNvPr id="2" name="Flecha: a la derecha 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F11EFA6-F96F-4D3C-A0D7-86F7F846B3A8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4F11EFA6-F96F-4D3C-A0D7-86F7F846B3A8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2446,7 +2446,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2456,8 +2456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M95"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A61" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52:I61"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -2475,152 +2475,152 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
     </row>
     <row r="2" spans="2:9" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="97" t="s">
+      <c r="B2" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="99"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="85"/>
     </row>
     <row r="3" spans="2:9" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="64"/>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="64"/>
+      <c r="B3" s="82"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
     </row>
     <row r="4" spans="2:9" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="64"/>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="64"/>
-      <c r="G4" s="64"/>
-      <c r="H4" s="64"/>
-      <c r="I4" s="64"/>
+      <c r="B4" s="82"/>
+      <c r="C4" s="82"/>
+      <c r="D4" s="82"/>
+      <c r="E4" s="82"/>
+      <c r="F4" s="82"/>
+      <c r="G4" s="82"/>
+      <c r="H4" s="82"/>
+      <c r="I4" s="82"/>
     </row>
     <row r="5" spans="2:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="B5" s="102" t="s">
+      <c r="B5" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="103"/>
-      <c r="D5" s="103"/>
-      <c r="E5" s="103"/>
-      <c r="F5" s="103"/>
-      <c r="G5" s="103"/>
-      <c r="H5" s="103"/>
-      <c r="I5" s="104"/>
+      <c r="C5" s="87"/>
+      <c r="D5" s="87"/>
+      <c r="E5" s="87"/>
+      <c r="F5" s="87"/>
+      <c r="G5" s="87"/>
+      <c r="H5" s="87"/>
+      <c r="I5" s="88"/>
     </row>
     <row r="6" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="100" t="s">
+      <c r="C6" s="59" t="s">
         <v>117</v>
       </c>
-      <c r="D6" s="100"/>
-      <c r="E6" s="100"/>
-      <c r="F6" s="100"/>
-      <c r="G6" s="100"/>
-      <c r="H6" s="100"/>
-      <c r="I6" s="101"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="59"/>
+      <c r="G6" s="59"/>
+      <c r="H6" s="59"/>
+      <c r="I6" s="60"/>
     </row>
     <row r="7" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B7" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="100" t="s">
+      <c r="C7" s="59" t="s">
         <v>64</v>
       </c>
-      <c r="D7" s="100"/>
-      <c r="E7" s="100"/>
-      <c r="F7" s="100"/>
-      <c r="G7" s="100"/>
-      <c r="H7" s="100"/>
-      <c r="I7" s="101"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="59"/>
+      <c r="F7" s="59"/>
+      <c r="G7" s="59"/>
+      <c r="H7" s="59"/>
+      <c r="I7" s="60"/>
     </row>
     <row r="8" spans="2:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="B8" s="125" t="s">
+      <c r="B8" s="78" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="100"/>
-      <c r="E8" s="100"/>
-      <c r="F8" s="100"/>
-      <c r="G8" s="100"/>
-      <c r="H8" s="100"/>
-      <c r="I8" s="101"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="59"/>
+      <c r="G8" s="59"/>
+      <c r="H8" s="59"/>
+      <c r="I8" s="60"/>
     </row>
     <row r="9" spans="2:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="B9" s="125"/>
+      <c r="B9" s="78"/>
       <c r="C9" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="100"/>
-      <c r="E9" s="100"/>
-      <c r="F9" s="100"/>
-      <c r="G9" s="100"/>
-      <c r="H9" s="100"/>
-      <c r="I9" s="101"/>
+      <c r="D9" s="59"/>
+      <c r="E9" s="59"/>
+      <c r="F9" s="59"/>
+      <c r="G9" s="59"/>
+      <c r="H9" s="59"/>
+      <c r="I9" s="60"/>
     </row>
     <row r="10" spans="2:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="B10" s="125"/>
+      <c r="B10" s="78"/>
       <c r="C10" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="100"/>
-      <c r="E10" s="100"/>
-      <c r="F10" s="100"/>
-      <c r="G10" s="100"/>
-      <c r="H10" s="100"/>
-      <c r="I10" s="101"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="59"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="59"/>
+      <c r="H10" s="59"/>
+      <c r="I10" s="60"/>
     </row>
     <row r="11" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B11" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="100" t="s">
+      <c r="C11" s="59" t="s">
         <v>65</v>
       </c>
-      <c r="D11" s="100"/>
-      <c r="E11" s="100"/>
-      <c r="F11" s="100"/>
-      <c r="G11" s="100"/>
-      <c r="H11" s="100"/>
-      <c r="I11" s="101"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="59"/>
+      <c r="G11" s="59"/>
+      <c r="H11" s="59"/>
+      <c r="I11" s="60"/>
     </row>
     <row r="12" spans="2:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="110" t="s">
+      <c r="C12" s="61" t="s">
         <v>117</v>
       </c>
-      <c r="D12" s="111"/>
-      <c r="E12" s="111"/>
-      <c r="F12" s="111"/>
-      <c r="G12" s="111"/>
-      <c r="H12" s="111"/>
-      <c r="I12" s="112"/>
+      <c r="D12" s="62"/>
+      <c r="E12" s="62"/>
+      <c r="F12" s="62"/>
+      <c r="G12" s="62"/>
+      <c r="H12" s="62"/>
+      <c r="I12" s="63"/>
     </row>
     <row r="13" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="2:9" ht="15" x14ac:dyDescent="0.25">
@@ -2636,76 +2636,76 @@
       <c r="I14" s="19"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="113" t="s">
+      <c r="B15" s="64" t="s">
         <v>116</v>
       </c>
-      <c r="C15" s="114"/>
-      <c r="D15" s="114"/>
-      <c r="E15" s="114"/>
-      <c r="F15" s="114"/>
-      <c r="G15" s="114"/>
-      <c r="H15" s="114"/>
-      <c r="I15" s="115"/>
+      <c r="C15" s="65"/>
+      <c r="D15" s="65"/>
+      <c r="E15" s="65"/>
+      <c r="F15" s="65"/>
+      <c r="G15" s="65"/>
+      <c r="H15" s="65"/>
+      <c r="I15" s="66"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="113"/>
-      <c r="C16" s="114"/>
-      <c r="D16" s="114"/>
-      <c r="E16" s="114"/>
-      <c r="F16" s="114"/>
-      <c r="G16" s="114"/>
-      <c r="H16" s="114"/>
-      <c r="I16" s="115"/>
+      <c r="B16" s="64"/>
+      <c r="C16" s="65"/>
+      <c r="D16" s="65"/>
+      <c r="E16" s="65"/>
+      <c r="F16" s="65"/>
+      <c r="G16" s="65"/>
+      <c r="H16" s="65"/>
+      <c r="I16" s="66"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="113"/>
-      <c r="C17" s="114"/>
-      <c r="D17" s="114"/>
-      <c r="E17" s="114"/>
-      <c r="F17" s="114"/>
-      <c r="G17" s="114"/>
-      <c r="H17" s="114"/>
-      <c r="I17" s="115"/>
+      <c r="B17" s="64"/>
+      <c r="C17" s="65"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="65"/>
+      <c r="F17" s="65"/>
+      <c r="G17" s="65"/>
+      <c r="H17" s="65"/>
+      <c r="I17" s="66"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="113"/>
-      <c r="C18" s="114"/>
-      <c r="D18" s="114"/>
-      <c r="E18" s="114"/>
-      <c r="F18" s="114"/>
-      <c r="G18" s="114"/>
-      <c r="H18" s="114"/>
-      <c r="I18" s="115"/>
+      <c r="B18" s="64"/>
+      <c r="C18" s="65"/>
+      <c r="D18" s="65"/>
+      <c r="E18" s="65"/>
+      <c r="F18" s="65"/>
+      <c r="G18" s="65"/>
+      <c r="H18" s="65"/>
+      <c r="I18" s="66"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="113"/>
-      <c r="C19" s="114"/>
-      <c r="D19" s="114"/>
-      <c r="E19" s="114"/>
-      <c r="F19" s="114"/>
-      <c r="G19" s="114"/>
-      <c r="H19" s="114"/>
-      <c r="I19" s="115"/>
+      <c r="B19" s="64"/>
+      <c r="C19" s="65"/>
+      <c r="D19" s="65"/>
+      <c r="E19" s="65"/>
+      <c r="F19" s="65"/>
+      <c r="G19" s="65"/>
+      <c r="H19" s="65"/>
+      <c r="I19" s="66"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="113"/>
-      <c r="C20" s="114"/>
-      <c r="D20" s="114"/>
-      <c r="E20" s="114"/>
-      <c r="F20" s="114"/>
-      <c r="G20" s="114"/>
-      <c r="H20" s="114"/>
-      <c r="I20" s="115"/>
+      <c r="B20" s="64"/>
+      <c r="C20" s="65"/>
+      <c r="D20" s="65"/>
+      <c r="E20" s="65"/>
+      <c r="F20" s="65"/>
+      <c r="G20" s="65"/>
+      <c r="H20" s="65"/>
+      <c r="I20" s="66"/>
     </row>
     <row r="21" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="116"/>
-      <c r="C21" s="117"/>
-      <c r="D21" s="117"/>
-      <c r="E21" s="117"/>
-      <c r="F21" s="117"/>
-      <c r="G21" s="117"/>
-      <c r="H21" s="117"/>
-      <c r="I21" s="118"/>
+      <c r="B21" s="67"/>
+      <c r="C21" s="68"/>
+      <c r="D21" s="68"/>
+      <c r="E21" s="68"/>
+      <c r="F21" s="68"/>
+      <c r="G21" s="68"/>
+      <c r="H21" s="68"/>
+      <c r="I21" s="69"/>
     </row>
     <row r="22" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="20"/>
@@ -2718,54 +2718,54 @@
       <c r="I22" s="20"/>
     </row>
     <row r="23" spans="2:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="B23" s="119" t="s">
+      <c r="B23" s="70" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="120"/>
-      <c r="D23" s="120"/>
-      <c r="E23" s="120"/>
-      <c r="F23" s="120"/>
-      <c r="G23" s="120"/>
-      <c r="H23" s="120"/>
-      <c r="I23" s="121"/>
+      <c r="C23" s="71"/>
+      <c r="D23" s="71"/>
+      <c r="E23" s="71"/>
+      <c r="F23" s="71"/>
+      <c r="G23" s="71"/>
+      <c r="H23" s="71"/>
+      <c r="I23" s="72"/>
     </row>
     <row r="24" spans="2:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="B24" s="107" t="s">
+      <c r="B24" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="108"/>
-      <c r="D24" s="108"/>
-      <c r="E24" s="108"/>
-      <c r="F24" s="109" t="s">
+      <c r="C24" s="57"/>
+      <c r="D24" s="57"/>
+      <c r="E24" s="57"/>
+      <c r="F24" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="G24" s="109"/>
-      <c r="H24" s="109"/>
+      <c r="G24" s="58"/>
+      <c r="H24" s="58"/>
       <c r="I24" s="25" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="25" spans="2:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="122" t="s">
+      <c r="B25" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="123"/>
-      <c r="D25" s="123"/>
-      <c r="E25" s="123"/>
-      <c r="F25" s="123"/>
-      <c r="G25" s="123"/>
-      <c r="H25" s="123"/>
-      <c r="I25" s="124"/>
+      <c r="C25" s="74"/>
+      <c r="D25" s="74"/>
+      <c r="E25" s="74"/>
+      <c r="F25" s="74"/>
+      <c r="G25" s="74"/>
+      <c r="H25" s="74"/>
+      <c r="I25" s="75"/>
     </row>
     <row r="26" spans="2:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="B26" s="95" t="s">
+      <c r="B26" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="C26" s="96"/>
-      <c r="D26" s="96" t="s">
+      <c r="C26" s="77"/>
+      <c r="D26" s="77" t="s">
         <v>17</v>
       </c>
-      <c r="E26" s="96"/>
+      <c r="E26" s="77"/>
       <c r="F26" s="23" t="s">
         <v>18</v>
       </c>
@@ -2780,14 +2780,14 @@
       </c>
     </row>
     <row r="27" spans="2:9" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="B27" s="57" t="s">
+      <c r="B27" s="79" t="s">
         <v>67</v>
       </c>
-      <c r="C27" s="58"/>
-      <c r="D27" s="58" t="s">
+      <c r="C27" s="80"/>
+      <c r="D27" s="80" t="s">
         <v>69</v>
       </c>
-      <c r="E27" s="58"/>
+      <c r="E27" s="80"/>
       <c r="F27" s="28">
         <v>3</v>
       </c>
@@ -2803,14 +2803,14 @@
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="57" t="s">
+      <c r="B28" s="79" t="s">
         <v>66</v>
       </c>
-      <c r="C28" s="58"/>
-      <c r="D28" s="94" t="s">
+      <c r="C28" s="80"/>
+      <c r="D28" s="81" t="s">
         <v>70</v>
       </c>
-      <c r="E28" s="94"/>
+      <c r="E28" s="81"/>
       <c r="F28" s="28">
         <v>3</v>
       </c>
@@ -2826,14 +2826,14 @@
       </c>
     </row>
     <row r="29" spans="2:9" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="B29" s="57" t="s">
+      <c r="B29" s="79" t="s">
         <v>84</v>
       </c>
-      <c r="C29" s="58"/>
-      <c r="D29" s="58" t="s">
+      <c r="C29" s="80"/>
+      <c r="D29" s="80" t="s">
         <v>71</v>
       </c>
-      <c r="E29" s="58"/>
+      <c r="E29" s="80"/>
       <c r="F29" s="28">
         <v>2</v>
       </c>
@@ -2849,14 +2849,14 @@
       </c>
     </row>
     <row r="30" spans="2:9" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="B30" s="57" t="s">
+      <c r="B30" s="79" t="s">
         <v>68</v>
       </c>
-      <c r="C30" s="94"/>
-      <c r="D30" s="58" t="s">
+      <c r="C30" s="81"/>
+      <c r="D30" s="80" t="s">
         <v>72</v>
       </c>
-      <c r="E30" s="58"/>
+      <c r="E30" s="80"/>
       <c r="F30" s="28">
         <v>3</v>
       </c>
@@ -2872,14 +2872,14 @@
       </c>
     </row>
     <row r="31" spans="2:9" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="B31" s="57" t="s">
+      <c r="B31" s="79" t="s">
         <v>85</v>
       </c>
-      <c r="C31" s="58"/>
-      <c r="D31" s="94" t="s">
+      <c r="C31" s="80"/>
+      <c r="D31" s="81" t="s">
         <v>87</v>
       </c>
-      <c r="E31" s="94"/>
+      <c r="E31" s="81"/>
       <c r="F31" s="28">
         <v>3</v>
       </c>
@@ -2895,14 +2895,14 @@
       </c>
     </row>
     <row r="32" spans="2:9" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="B32" s="93" t="s">
+      <c r="B32" s="90" t="s">
         <v>86</v>
       </c>
-      <c r="C32" s="94"/>
-      <c r="D32" s="58" t="s">
+      <c r="C32" s="81"/>
+      <c r="D32" s="80" t="s">
         <v>90</v>
       </c>
-      <c r="E32" s="58"/>
+      <c r="E32" s="80"/>
       <c r="F32" s="28">
         <v>3</v>
       </c>
@@ -2930,14 +2930,14 @@
       </c>
     </row>
     <row r="34" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="95" t="s">
+      <c r="B34" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="C34" s="96"/>
-      <c r="D34" s="96" t="s">
+      <c r="C34" s="77"/>
+      <c r="D34" s="77" t="s">
         <v>17</v>
       </c>
-      <c r="E34" s="96"/>
+      <c r="E34" s="77"/>
       <c r="F34" s="23" t="s">
         <v>18</v>
       </c>
@@ -2950,22 +2950,22 @@
       <c r="I34" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="J34" s="54" t="s">
+      <c r="J34" s="114" t="s">
         <v>23</v>
       </c>
-      <c r="K34" s="55"/>
-      <c r="L34" s="55"/>
-      <c r="M34" s="56"/>
+      <c r="K34" s="115"/>
+      <c r="L34" s="115"/>
+      <c r="M34" s="116"/>
     </row>
     <row r="35" spans="2:13" s="3" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="93" t="s">
+      <c r="B35" s="90" t="s">
         <v>77</v>
       </c>
-      <c r="C35" s="94"/>
-      <c r="D35" s="94" t="s">
+      <c r="C35" s="81"/>
+      <c r="D35" s="81" t="s">
         <v>78</v>
       </c>
-      <c r="E35" s="94"/>
+      <c r="E35" s="81"/>
       <c r="F35" s="28">
         <v>2</v>
       </c>
@@ -2979,20 +2979,20 @@
       <c r="I35" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="J35" s="63"/>
-      <c r="K35" s="64"/>
-      <c r="L35" s="64"/>
-      <c r="M35" s="65"/>
+      <c r="J35" s="117"/>
+      <c r="K35" s="82"/>
+      <c r="L35" s="82"/>
+      <c r="M35" s="118"/>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B36" s="93" t="s">
+      <c r="B36" s="90" t="s">
         <v>79</v>
       </c>
-      <c r="C36" s="94"/>
-      <c r="D36" s="94" t="s">
+      <c r="C36" s="81"/>
+      <c r="D36" s="81" t="s">
         <v>94</v>
       </c>
-      <c r="E36" s="94"/>
+      <c r="E36" s="81"/>
       <c r="F36" s="28">
         <v>3</v>
       </c>
@@ -3008,14 +3008,14 @@
       </c>
     </row>
     <row r="37" spans="2:13" s="3" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="93" t="s">
+      <c r="B37" s="90" t="s">
         <v>80</v>
       </c>
-      <c r="C37" s="94"/>
-      <c r="D37" s="94" t="s">
+      <c r="C37" s="81"/>
+      <c r="D37" s="81" t="s">
         <v>82</v>
       </c>
-      <c r="E37" s="94"/>
+      <c r="E37" s="81"/>
       <c r="F37" s="28">
         <v>3</v>
       </c>
@@ -3029,20 +3029,20 @@
       <c r="I37" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="J37" s="63"/>
-      <c r="K37" s="64"/>
-      <c r="L37" s="64"/>
-      <c r="M37" s="65"/>
+      <c r="J37" s="117"/>
+      <c r="K37" s="82"/>
+      <c r="L37" s="82"/>
+      <c r="M37" s="118"/>
     </row>
     <row r="38" spans="2:13" s="3" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="93" t="s">
+      <c r="B38" s="90" t="s">
         <v>91</v>
       </c>
-      <c r="C38" s="94"/>
-      <c r="D38" s="94" t="s">
+      <c r="C38" s="81"/>
+      <c r="D38" s="81" t="s">
         <v>92</v>
       </c>
-      <c r="E38" s="94"/>
+      <c r="E38" s="81"/>
       <c r="F38" s="28">
         <v>3</v>
       </c>
@@ -3056,16 +3056,16 @@
       <c r="I38" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="J38" s="63"/>
-      <c r="K38" s="64"/>
-      <c r="L38" s="64"/>
-      <c r="M38" s="65"/>
+      <c r="J38" s="117"/>
+      <c r="K38" s="82"/>
+      <c r="L38" s="82"/>
+      <c r="M38" s="118"/>
     </row>
     <row r="39" spans="2:13" s="3" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="87"/>
-      <c r="C39" s="88"/>
-      <c r="D39" s="88"/>
-      <c r="E39" s="88"/>
+      <c r="B39" s="125"/>
+      <c r="C39" s="91"/>
+      <c r="D39" s="91"/>
+      <c r="E39" s="91"/>
       <c r="F39" s="11"/>
       <c r="G39" s="11"/>
       <c r="H39" s="11">
@@ -3073,10 +3073,10 @@
         <v>0</v>
       </c>
       <c r="I39" s="5"/>
-      <c r="J39" s="66"/>
-      <c r="K39" s="67"/>
-      <c r="L39" s="67"/>
-      <c r="M39" s="68"/>
+      <c r="J39" s="119"/>
+      <c r="K39" s="120"/>
+      <c r="L39" s="120"/>
+      <c r="M39" s="121"/>
     </row>
     <row r="40" spans="2:13" s="3" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="41" spans="2:13" ht="15" x14ac:dyDescent="0.25">
@@ -3093,11 +3093,11 @@
     </row>
     <row r="42" spans="2:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="9"/>
-      <c r="C42" s="91" t="s">
+      <c r="C42" s="95" t="s">
         <v>25</v>
       </c>
-      <c r="D42" s="91"/>
-      <c r="E42" s="91"/>
+      <c r="D42" s="95"/>
+      <c r="E42" s="95"/>
       <c r="F42" s="26" t="s">
         <v>26</v>
       </c>
@@ -3110,81 +3110,81 @@
       <c r="I42" s="10"/>
     </row>
     <row r="43" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="73" t="s">
+      <c r="B43" s="92" t="s">
         <v>29</v>
       </c>
-      <c r="C43" s="92" t="s">
+      <c r="C43" s="96" t="s">
         <v>118</v>
       </c>
-      <c r="D43" s="74"/>
-      <c r="E43" s="74"/>
-      <c r="F43" s="72" t="s">
+      <c r="D43" s="97"/>
+      <c r="E43" s="97"/>
+      <c r="F43" s="89" t="s">
         <v>96</v>
       </c>
-      <c r="G43" s="72"/>
-      <c r="H43" s="72"/>
+      <c r="G43" s="89"/>
+      <c r="H43" s="89"/>
       <c r="I43" s="10"/>
     </row>
     <row r="44" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="73"/>
-      <c r="C44" s="74"/>
-      <c r="D44" s="74"/>
-      <c r="E44" s="74"/>
-      <c r="F44" s="72"/>
-      <c r="G44" s="72"/>
-      <c r="H44" s="72"/>
+      <c r="B44" s="92"/>
+      <c r="C44" s="97"/>
+      <c r="D44" s="97"/>
+      <c r="E44" s="97"/>
+      <c r="F44" s="89"/>
+      <c r="G44" s="89"/>
+      <c r="H44" s="89"/>
       <c r="I44" s="10"/>
     </row>
     <row r="45" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="73" t="s">
+      <c r="B45" s="92" t="s">
         <v>30</v>
       </c>
-      <c r="C45" s="89" t="s">
+      <c r="C45" s="93" t="s">
         <v>119</v>
       </c>
-      <c r="D45" s="90"/>
-      <c r="E45" s="90"/>
-      <c r="F45" s="72"/>
-      <c r="G45" s="72" t="s">
+      <c r="D45" s="94"/>
+      <c r="E45" s="94"/>
+      <c r="F45" s="89"/>
+      <c r="G45" s="89" t="s">
         <v>96</v>
       </c>
-      <c r="H45" s="72"/>
+      <c r="H45" s="89"/>
       <c r="I45" s="10"/>
     </row>
     <row r="46" spans="2:13" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="73"/>
-      <c r="C46" s="90"/>
-      <c r="D46" s="90"/>
-      <c r="E46" s="90"/>
-      <c r="F46" s="72"/>
-      <c r="G46" s="72"/>
-      <c r="H46" s="72"/>
+      <c r="B46" s="92"/>
+      <c r="C46" s="94"/>
+      <c r="D46" s="94"/>
+      <c r="E46" s="94"/>
+      <c r="F46" s="89"/>
+      <c r="G46" s="89"/>
+      <c r="H46" s="89"/>
       <c r="I46" s="10"/>
     </row>
     <row r="47" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="73" t="s">
+      <c r="B47" s="92" t="s">
         <v>31</v>
       </c>
-      <c r="C47" s="74" t="s">
+      <c r="C47" s="97" t="s">
         <v>120</v>
       </c>
-      <c r="D47" s="74"/>
-      <c r="E47" s="74"/>
-      <c r="F47" s="72" t="s">
+      <c r="D47" s="97"/>
+      <c r="E47" s="97"/>
+      <c r="F47" s="89" t="s">
         <v>96</v>
       </c>
-      <c r="G47" s="72"/>
-      <c r="H47" s="72"/>
+      <c r="G47" s="89"/>
+      <c r="H47" s="89"/>
       <c r="I47" s="10"/>
     </row>
     <row r="48" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="73"/>
-      <c r="C48" s="74"/>
-      <c r="D48" s="74"/>
-      <c r="E48" s="74"/>
-      <c r="F48" s="72"/>
-      <c r="G48" s="72"/>
-      <c r="H48" s="72"/>
+      <c r="B48" s="92"/>
+      <c r="C48" s="97"/>
+      <c r="D48" s="97"/>
+      <c r="E48" s="97"/>
+      <c r="F48" s="89"/>
+      <c r="G48" s="89"/>
+      <c r="H48" s="89"/>
       <c r="I48" s="10"/>
     </row>
     <row r="49" spans="2:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3199,126 +3199,126 @@
     </row>
     <row r="50" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="51" spans="2:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="69" t="s">
+      <c r="B51" s="122" t="s">
         <v>32</v>
       </c>
-      <c r="C51" s="70"/>
-      <c r="D51" s="70"/>
-      <c r="E51" s="70"/>
-      <c r="F51" s="70"/>
-      <c r="G51" s="70"/>
-      <c r="H51" s="70"/>
-      <c r="I51" s="71"/>
+      <c r="C51" s="123"/>
+      <c r="D51" s="123"/>
+      <c r="E51" s="123"/>
+      <c r="F51" s="123"/>
+      <c r="G51" s="123"/>
+      <c r="H51" s="123"/>
+      <c r="I51" s="124"/>
     </row>
     <row r="52" spans="2:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="57"/>
-      <c r="C52" s="58"/>
-      <c r="D52" s="58"/>
-      <c r="E52" s="58"/>
-      <c r="F52" s="58"/>
-      <c r="G52" s="58"/>
-      <c r="H52" s="58"/>
-      <c r="I52" s="59"/>
+      <c r="B52" s="79"/>
+      <c r="C52" s="80"/>
+      <c r="D52" s="80"/>
+      <c r="E52" s="80"/>
+      <c r="F52" s="80"/>
+      <c r="G52" s="80"/>
+      <c r="H52" s="80"/>
+      <c r="I52" s="110"/>
     </row>
     <row r="53" spans="2:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="57"/>
-      <c r="C53" s="58"/>
-      <c r="D53" s="58"/>
-      <c r="E53" s="58"/>
-      <c r="F53" s="58"/>
-      <c r="G53" s="58"/>
-      <c r="H53" s="58"/>
-      <c r="I53" s="59"/>
+      <c r="B53" s="79"/>
+      <c r="C53" s="80"/>
+      <c r="D53" s="80"/>
+      <c r="E53" s="80"/>
+      <c r="F53" s="80"/>
+      <c r="G53" s="80"/>
+      <c r="H53" s="80"/>
+      <c r="I53" s="110"/>
     </row>
     <row r="54" spans="2:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="57"/>
-      <c r="C54" s="58"/>
-      <c r="D54" s="58"/>
-      <c r="E54" s="58"/>
-      <c r="F54" s="58"/>
-      <c r="G54" s="58"/>
-      <c r="H54" s="58"/>
-      <c r="I54" s="59"/>
+      <c r="B54" s="79"/>
+      <c r="C54" s="80"/>
+      <c r="D54" s="80"/>
+      <c r="E54" s="80"/>
+      <c r="F54" s="80"/>
+      <c r="G54" s="80"/>
+      <c r="H54" s="80"/>
+      <c r="I54" s="110"/>
     </row>
     <row r="55" spans="2:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="57"/>
-      <c r="C55" s="58"/>
-      <c r="D55" s="58"/>
-      <c r="E55" s="58"/>
-      <c r="F55" s="58"/>
-      <c r="G55" s="58"/>
-      <c r="H55" s="58"/>
-      <c r="I55" s="59"/>
+      <c r="B55" s="79"/>
+      <c r="C55" s="80"/>
+      <c r="D55" s="80"/>
+      <c r="E55" s="80"/>
+      <c r="F55" s="80"/>
+      <c r="G55" s="80"/>
+      <c r="H55" s="80"/>
+      <c r="I55" s="110"/>
     </row>
     <row r="56" spans="2:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="57"/>
-      <c r="C56" s="58"/>
-      <c r="D56" s="58"/>
-      <c r="E56" s="58"/>
-      <c r="F56" s="58"/>
-      <c r="G56" s="58"/>
-      <c r="H56" s="58"/>
-      <c r="I56" s="59"/>
+      <c r="B56" s="79"/>
+      <c r="C56" s="80"/>
+      <c r="D56" s="80"/>
+      <c r="E56" s="80"/>
+      <c r="F56" s="80"/>
+      <c r="G56" s="80"/>
+      <c r="H56" s="80"/>
+      <c r="I56" s="110"/>
     </row>
     <row r="57" spans="2:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="57"/>
-      <c r="C57" s="58"/>
-      <c r="D57" s="58"/>
-      <c r="E57" s="58"/>
-      <c r="F57" s="58"/>
-      <c r="G57" s="58"/>
-      <c r="H57" s="58"/>
-      <c r="I57" s="59"/>
+      <c r="B57" s="79"/>
+      <c r="C57" s="80"/>
+      <c r="D57" s="80"/>
+      <c r="E57" s="80"/>
+      <c r="F57" s="80"/>
+      <c r="G57" s="80"/>
+      <c r="H57" s="80"/>
+      <c r="I57" s="110"/>
     </row>
     <row r="58" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="57"/>
-      <c r="C58" s="58"/>
-      <c r="D58" s="58"/>
-      <c r="E58" s="58"/>
-      <c r="F58" s="58"/>
-      <c r="G58" s="58"/>
-      <c r="H58" s="58"/>
-      <c r="I58" s="59"/>
+      <c r="B58" s="79"/>
+      <c r="C58" s="80"/>
+      <c r="D58" s="80"/>
+      <c r="E58" s="80"/>
+      <c r="F58" s="80"/>
+      <c r="G58" s="80"/>
+      <c r="H58" s="80"/>
+      <c r="I58" s="110"/>
     </row>
     <row r="59" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="57"/>
-      <c r="C59" s="58"/>
-      <c r="D59" s="58"/>
-      <c r="E59" s="58"/>
-      <c r="F59" s="58"/>
-      <c r="G59" s="58"/>
-      <c r="H59" s="58"/>
-      <c r="I59" s="59"/>
+      <c r="B59" s="79"/>
+      <c r="C59" s="80"/>
+      <c r="D59" s="80"/>
+      <c r="E59" s="80"/>
+      <c r="F59" s="80"/>
+      <c r="G59" s="80"/>
+      <c r="H59" s="80"/>
+      <c r="I59" s="110"/>
     </row>
     <row r="60" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="57"/>
-      <c r="C60" s="58"/>
-      <c r="D60" s="58"/>
-      <c r="E60" s="58"/>
-      <c r="F60" s="58"/>
-      <c r="G60" s="58"/>
-      <c r="H60" s="58"/>
-      <c r="I60" s="59"/>
+      <c r="B60" s="79"/>
+      <c r="C60" s="80"/>
+      <c r="D60" s="80"/>
+      <c r="E60" s="80"/>
+      <c r="F60" s="80"/>
+      <c r="G60" s="80"/>
+      <c r="H60" s="80"/>
+      <c r="I60" s="110"/>
     </row>
     <row r="61" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="60"/>
-      <c r="C61" s="61"/>
-      <c r="D61" s="61"/>
-      <c r="E61" s="61"/>
-      <c r="F61" s="61"/>
-      <c r="G61" s="61"/>
-      <c r="H61" s="61"/>
-      <c r="I61" s="62"/>
+      <c r="B61" s="111"/>
+      <c r="C61" s="112"/>
+      <c r="D61" s="112"/>
+      <c r="E61" s="112"/>
+      <c r="F61" s="112"/>
+      <c r="G61" s="112"/>
+      <c r="H61" s="112"/>
+      <c r="I61" s="113"/>
     </row>
     <row r="62" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="64"/>
-      <c r="C62" s="64"/>
-      <c r="D62" s="64"/>
-      <c r="E62" s="64"/>
-      <c r="F62" s="64"/>
-      <c r="G62" s="64"/>
-      <c r="H62" s="64"/>
-      <c r="I62" s="64"/>
+      <c r="B62" s="82"/>
+      <c r="C62" s="82"/>
+      <c r="D62" s="82"/>
+      <c r="E62" s="82"/>
+      <c r="F62" s="82"/>
+      <c r="G62" s="82"/>
+      <c r="H62" s="82"/>
+      <c r="I62" s="82"/>
     </row>
     <row r="63" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B63" s="17" t="s">
@@ -3333,200 +3333,200 @@
       <c r="I63" s="19"/>
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B64" s="75" t="s">
+      <c r="B64" s="98" t="s">
         <v>34</v>
       </c>
-      <c r="C64" s="76"/>
-      <c r="D64" s="76"/>
-      <c r="E64" s="76"/>
-      <c r="F64" s="76"/>
-      <c r="G64" s="76"/>
-      <c r="H64" s="76"/>
-      <c r="I64" s="77"/>
+      <c r="C64" s="99"/>
+      <c r="D64" s="99"/>
+      <c r="E64" s="99"/>
+      <c r="F64" s="99"/>
+      <c r="G64" s="99"/>
+      <c r="H64" s="99"/>
+      <c r="I64" s="100"/>
     </row>
     <row r="65" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="57"/>
-      <c r="C65" s="58"/>
-      <c r="D65" s="58"/>
-      <c r="E65" s="58"/>
-      <c r="F65" s="58"/>
-      <c r="G65" s="58"/>
-      <c r="H65" s="58"/>
-      <c r="I65" s="59"/>
+      <c r="B65" s="79"/>
+      <c r="C65" s="80"/>
+      <c r="D65" s="80"/>
+      <c r="E65" s="80"/>
+      <c r="F65" s="80"/>
+      <c r="G65" s="80"/>
+      <c r="H65" s="80"/>
+      <c r="I65" s="110"/>
     </row>
     <row r="66" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="57"/>
-      <c r="C66" s="58"/>
-      <c r="D66" s="58"/>
-      <c r="E66" s="58"/>
-      <c r="F66" s="58"/>
-      <c r="G66" s="58"/>
-      <c r="H66" s="58"/>
-      <c r="I66" s="59"/>
+      <c r="B66" s="79"/>
+      <c r="C66" s="80"/>
+      <c r="D66" s="80"/>
+      <c r="E66" s="80"/>
+      <c r="F66" s="80"/>
+      <c r="G66" s="80"/>
+      <c r="H66" s="80"/>
+      <c r="I66" s="110"/>
     </row>
     <row r="67" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="57"/>
-      <c r="C67" s="58"/>
-      <c r="D67" s="58"/>
-      <c r="E67" s="58"/>
-      <c r="F67" s="58"/>
-      <c r="G67" s="58"/>
-      <c r="H67" s="58"/>
-      <c r="I67" s="59"/>
+      <c r="B67" s="79"/>
+      <c r="C67" s="80"/>
+      <c r="D67" s="80"/>
+      <c r="E67" s="80"/>
+      <c r="F67" s="80"/>
+      <c r="G67" s="80"/>
+      <c r="H67" s="80"/>
+      <c r="I67" s="110"/>
     </row>
     <row r="68" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="57"/>
-      <c r="C68" s="58"/>
-      <c r="D68" s="58"/>
-      <c r="E68" s="58"/>
-      <c r="F68" s="58"/>
-      <c r="G68" s="58"/>
-      <c r="H68" s="58"/>
-      <c r="I68" s="59"/>
+      <c r="B68" s="79"/>
+      <c r="C68" s="80"/>
+      <c r="D68" s="80"/>
+      <c r="E68" s="80"/>
+      <c r="F68" s="80"/>
+      <c r="G68" s="80"/>
+      <c r="H68" s="80"/>
+      <c r="I68" s="110"/>
     </row>
     <row r="69" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="57"/>
-      <c r="C69" s="58"/>
-      <c r="D69" s="58"/>
-      <c r="E69" s="58"/>
-      <c r="F69" s="58"/>
-      <c r="G69" s="58"/>
-      <c r="H69" s="58"/>
-      <c r="I69" s="59"/>
+      <c r="B69" s="79"/>
+      <c r="C69" s="80"/>
+      <c r="D69" s="80"/>
+      <c r="E69" s="80"/>
+      <c r="F69" s="80"/>
+      <c r="G69" s="80"/>
+      <c r="H69" s="80"/>
+      <c r="I69" s="110"/>
     </row>
     <row r="70" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="57"/>
-      <c r="C70" s="58"/>
-      <c r="D70" s="58"/>
-      <c r="E70" s="58"/>
-      <c r="F70" s="58"/>
-      <c r="G70" s="58"/>
-      <c r="H70" s="58"/>
-      <c r="I70" s="59"/>
+      <c r="B70" s="79"/>
+      <c r="C70" s="80"/>
+      <c r="D70" s="80"/>
+      <c r="E70" s="80"/>
+      <c r="F70" s="80"/>
+      <c r="G70" s="80"/>
+      <c r="H70" s="80"/>
+      <c r="I70" s="110"/>
     </row>
     <row r="71" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="57"/>
-      <c r="C71" s="58"/>
-      <c r="D71" s="58"/>
-      <c r="E71" s="58"/>
-      <c r="F71" s="58"/>
-      <c r="G71" s="58"/>
-      <c r="H71" s="58"/>
-      <c r="I71" s="59"/>
+      <c r="B71" s="79"/>
+      <c r="C71" s="80"/>
+      <c r="D71" s="80"/>
+      <c r="E71" s="80"/>
+      <c r="F71" s="80"/>
+      <c r="G71" s="80"/>
+      <c r="H71" s="80"/>
+      <c r="I71" s="110"/>
     </row>
     <row r="72" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="57"/>
-      <c r="C72" s="58"/>
-      <c r="D72" s="58"/>
-      <c r="E72" s="58"/>
-      <c r="F72" s="58"/>
-      <c r="G72" s="58"/>
-      <c r="H72" s="58"/>
-      <c r="I72" s="59"/>
+      <c r="B72" s="79"/>
+      <c r="C72" s="80"/>
+      <c r="D72" s="80"/>
+      <c r="E72" s="80"/>
+      <c r="F72" s="80"/>
+      <c r="G72" s="80"/>
+      <c r="H72" s="80"/>
+      <c r="I72" s="110"/>
     </row>
     <row r="73" spans="2:9" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="57"/>
-      <c r="C73" s="58"/>
-      <c r="D73" s="58"/>
-      <c r="E73" s="58"/>
-      <c r="F73" s="58"/>
-      <c r="G73" s="58"/>
-      <c r="H73" s="58"/>
-      <c r="I73" s="59"/>
+      <c r="B73" s="79"/>
+      <c r="C73" s="80"/>
+      <c r="D73" s="80"/>
+      <c r="E73" s="80"/>
+      <c r="F73" s="80"/>
+      <c r="G73" s="80"/>
+      <c r="H73" s="80"/>
+      <c r="I73" s="110"/>
     </row>
     <row r="74" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B74" s="75" t="s">
+      <c r="B74" s="98" t="s">
         <v>35</v>
       </c>
-      <c r="C74" s="76"/>
-      <c r="D74" s="76"/>
-      <c r="E74" s="76"/>
-      <c r="F74" s="76"/>
-      <c r="G74" s="76"/>
-      <c r="H74" s="76"/>
-      <c r="I74" s="77"/>
+      <c r="C74" s="99"/>
+      <c r="D74" s="99"/>
+      <c r="E74" s="99"/>
+      <c r="F74" s="99"/>
+      <c r="G74" s="99"/>
+      <c r="H74" s="99"/>
+      <c r="I74" s="100"/>
     </row>
     <row r="75" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B75" s="57" t="s">
+      <c r="B75" s="79" t="s">
         <v>121</v>
       </c>
-      <c r="C75" s="58"/>
-      <c r="D75" s="58"/>
-      <c r="E75" s="58"/>
-      <c r="F75" s="58"/>
-      <c r="G75" s="58"/>
-      <c r="H75" s="58"/>
-      <c r="I75" s="59"/>
+      <c r="C75" s="80"/>
+      <c r="D75" s="80"/>
+      <c r="E75" s="80"/>
+      <c r="F75" s="80"/>
+      <c r="G75" s="80"/>
+      <c r="H75" s="80"/>
+      <c r="I75" s="110"/>
     </row>
     <row r="76" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B76" s="57"/>
-      <c r="C76" s="58"/>
-      <c r="D76" s="58"/>
-      <c r="E76" s="58"/>
-      <c r="F76" s="58"/>
-      <c r="G76" s="58"/>
-      <c r="H76" s="58"/>
-      <c r="I76" s="59"/>
+      <c r="B76" s="79"/>
+      <c r="C76" s="80"/>
+      <c r="D76" s="80"/>
+      <c r="E76" s="80"/>
+      <c r="F76" s="80"/>
+      <c r="G76" s="80"/>
+      <c r="H76" s="80"/>
+      <c r="I76" s="110"/>
     </row>
     <row r="77" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B77" s="57"/>
-      <c r="C77" s="58"/>
-      <c r="D77" s="58"/>
-      <c r="E77" s="58"/>
-      <c r="F77" s="58"/>
-      <c r="G77" s="58"/>
-      <c r="H77" s="58"/>
-      <c r="I77" s="59"/>
+      <c r="B77" s="79"/>
+      <c r="C77" s="80"/>
+      <c r="D77" s="80"/>
+      <c r="E77" s="80"/>
+      <c r="F77" s="80"/>
+      <c r="G77" s="80"/>
+      <c r="H77" s="80"/>
+      <c r="I77" s="110"/>
     </row>
     <row r="78" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B78" s="57"/>
-      <c r="C78" s="58"/>
-      <c r="D78" s="58"/>
-      <c r="E78" s="58"/>
-      <c r="F78" s="58"/>
-      <c r="G78" s="58"/>
-      <c r="H78" s="58"/>
-      <c r="I78" s="59"/>
+      <c r="B78" s="79"/>
+      <c r="C78" s="80"/>
+      <c r="D78" s="80"/>
+      <c r="E78" s="80"/>
+      <c r="F78" s="80"/>
+      <c r="G78" s="80"/>
+      <c r="H78" s="80"/>
+      <c r="I78" s="110"/>
     </row>
     <row r="79" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B79" s="57"/>
-      <c r="C79" s="58"/>
-      <c r="D79" s="58"/>
-      <c r="E79" s="58"/>
-      <c r="F79" s="58"/>
-      <c r="G79" s="58"/>
-      <c r="H79" s="58"/>
-      <c r="I79" s="59"/>
+      <c r="B79" s="79"/>
+      <c r="C79" s="80"/>
+      <c r="D79" s="80"/>
+      <c r="E79" s="80"/>
+      <c r="F79" s="80"/>
+      <c r="G79" s="80"/>
+      <c r="H79" s="80"/>
+      <c r="I79" s="110"/>
     </row>
     <row r="80" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B80" s="57"/>
-      <c r="C80" s="58"/>
-      <c r="D80" s="58"/>
-      <c r="E80" s="58"/>
-      <c r="F80" s="58"/>
-      <c r="G80" s="58"/>
-      <c r="H80" s="58"/>
-      <c r="I80" s="59"/>
+      <c r="B80" s="79"/>
+      <c r="C80" s="80"/>
+      <c r="D80" s="80"/>
+      <c r="E80" s="80"/>
+      <c r="F80" s="80"/>
+      <c r="G80" s="80"/>
+      <c r="H80" s="80"/>
+      <c r="I80" s="110"/>
     </row>
     <row r="81" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B81" s="57"/>
-      <c r="C81" s="58"/>
-      <c r="D81" s="58"/>
-      <c r="E81" s="58"/>
-      <c r="F81" s="58"/>
-      <c r="G81" s="58"/>
-      <c r="H81" s="58"/>
-      <c r="I81" s="59"/>
+      <c r="B81" s="79"/>
+      <c r="C81" s="80"/>
+      <c r="D81" s="80"/>
+      <c r="E81" s="80"/>
+      <c r="F81" s="80"/>
+      <c r="G81" s="80"/>
+      <c r="H81" s="80"/>
+      <c r="I81" s="110"/>
     </row>
     <row r="82" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B82" s="60"/>
-      <c r="C82" s="61"/>
-      <c r="D82" s="61"/>
-      <c r="E82" s="61"/>
-      <c r="F82" s="61"/>
-      <c r="G82" s="61"/>
-      <c r="H82" s="61"/>
-      <c r="I82" s="62"/>
+      <c r="B82" s="111"/>
+      <c r="C82" s="112"/>
+      <c r="D82" s="112"/>
+      <c r="E82" s="112"/>
+      <c r="F82" s="112"/>
+      <c r="G82" s="112"/>
+      <c r="H82" s="112"/>
+      <c r="I82" s="113"/>
     </row>
     <row r="84" spans="2:11" ht="15" x14ac:dyDescent="0.25">
       <c r="B84" s="6" t="s">
@@ -3553,113 +3553,172 @@
       <c r="I85" s="7"/>
     </row>
     <row r="86" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B86" s="78" t="s">
+      <c r="B86" s="101" t="s">
         <v>122</v>
       </c>
-      <c r="C86" s="79"/>
-      <c r="D86" s="79"/>
-      <c r="E86" s="79"/>
-      <c r="F86" s="79"/>
-      <c r="G86" s="79"/>
-      <c r="H86" s="79"/>
-      <c r="I86" s="80"/>
+      <c r="C86" s="102"/>
+      <c r="D86" s="102"/>
+      <c r="E86" s="102"/>
+      <c r="F86" s="102"/>
+      <c r="G86" s="102"/>
+      <c r="H86" s="102"/>
+      <c r="I86" s="103"/>
     </row>
     <row r="87" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B87" s="81"/>
-      <c r="C87" s="82"/>
-      <c r="D87" s="82"/>
-      <c r="E87" s="82"/>
-      <c r="F87" s="82"/>
-      <c r="G87" s="82"/>
-      <c r="H87" s="82"/>
-      <c r="I87" s="83"/>
+      <c r="B87" s="104"/>
+      <c r="C87" s="105"/>
+      <c r="D87" s="105"/>
+      <c r="E87" s="105"/>
+      <c r="F87" s="105"/>
+      <c r="G87" s="105"/>
+      <c r="H87" s="105"/>
+      <c r="I87" s="106"/>
     </row>
     <row r="88" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B88" s="81"/>
-      <c r="C88" s="82"/>
-      <c r="D88" s="82"/>
-      <c r="E88" s="82"/>
-      <c r="F88" s="82"/>
-      <c r="G88" s="82"/>
-      <c r="H88" s="82"/>
-      <c r="I88" s="83"/>
+      <c r="B88" s="104"/>
+      <c r="C88" s="105"/>
+      <c r="D88" s="105"/>
+      <c r="E88" s="105"/>
+      <c r="F88" s="105"/>
+      <c r="G88" s="105"/>
+      <c r="H88" s="105"/>
+      <c r="I88" s="106"/>
     </row>
     <row r="89" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B89" s="81"/>
-      <c r="C89" s="82"/>
-      <c r="D89" s="82"/>
-      <c r="E89" s="82"/>
-      <c r="F89" s="82"/>
-      <c r="G89" s="82"/>
-      <c r="H89" s="82"/>
-      <c r="I89" s="83"/>
+      <c r="B89" s="104"/>
+      <c r="C89" s="105"/>
+      <c r="D89" s="105"/>
+      <c r="E89" s="105"/>
+      <c r="F89" s="105"/>
+      <c r="G89" s="105"/>
+      <c r="H89" s="105"/>
+      <c r="I89" s="106"/>
     </row>
     <row r="90" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B90" s="81"/>
-      <c r="C90" s="82"/>
-      <c r="D90" s="82"/>
-      <c r="E90" s="82"/>
-      <c r="F90" s="82"/>
-      <c r="G90" s="82"/>
-      <c r="H90" s="82"/>
-      <c r="I90" s="83"/>
+      <c r="B90" s="104"/>
+      <c r="C90" s="105"/>
+      <c r="D90" s="105"/>
+      <c r="E90" s="105"/>
+      <c r="F90" s="105"/>
+      <c r="G90" s="105"/>
+      <c r="H90" s="105"/>
+      <c r="I90" s="106"/>
     </row>
     <row r="91" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B91" s="81"/>
-      <c r="C91" s="82"/>
-      <c r="D91" s="82"/>
-      <c r="E91" s="82"/>
-      <c r="F91" s="82"/>
-      <c r="G91" s="82"/>
-      <c r="H91" s="82"/>
-      <c r="I91" s="83"/>
+      <c r="B91" s="104"/>
+      <c r="C91" s="105"/>
+      <c r="D91" s="105"/>
+      <c r="E91" s="105"/>
+      <c r="F91" s="105"/>
+      <c r="G91" s="105"/>
+      <c r="H91" s="105"/>
+      <c r="I91" s="106"/>
     </row>
     <row r="92" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B92" s="81"/>
-      <c r="C92" s="82"/>
-      <c r="D92" s="82"/>
-      <c r="E92" s="82"/>
-      <c r="F92" s="82"/>
-      <c r="G92" s="82"/>
-      <c r="H92" s="82"/>
-      <c r="I92" s="83"/>
+      <c r="B92" s="104"/>
+      <c r="C92" s="105"/>
+      <c r="D92" s="105"/>
+      <c r="E92" s="105"/>
+      <c r="F92" s="105"/>
+      <c r="G92" s="105"/>
+      <c r="H92" s="105"/>
+      <c r="I92" s="106"/>
     </row>
     <row r="93" spans="2:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="B93" s="81"/>
-      <c r="C93" s="82"/>
-      <c r="D93" s="82"/>
-      <c r="E93" s="82"/>
-      <c r="F93" s="82"/>
-      <c r="G93" s="82"/>
-      <c r="H93" s="82"/>
-      <c r="I93" s="83"/>
-      <c r="J93" s="105" t="s">
+      <c r="B93" s="104"/>
+      <c r="C93" s="105"/>
+      <c r="D93" s="105"/>
+      <c r="E93" s="105"/>
+      <c r="F93" s="105"/>
+      <c r="G93" s="105"/>
+      <c r="H93" s="105"/>
+      <c r="I93" s="106"/>
+      <c r="J93" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="K93" s="106"/>
+      <c r="K93" s="55"/>
     </row>
     <row r="94" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B94" s="81"/>
-      <c r="C94" s="82"/>
-      <c r="D94" s="82"/>
-      <c r="E94" s="82"/>
-      <c r="F94" s="82"/>
-      <c r="G94" s="82"/>
-      <c r="H94" s="82"/>
-      <c r="I94" s="83"/>
+      <c r="B94" s="104"/>
+      <c r="C94" s="105"/>
+      <c r="D94" s="105"/>
+      <c r="E94" s="105"/>
+      <c r="F94" s="105"/>
+      <c r="G94" s="105"/>
+      <c r="H94" s="105"/>
+      <c r="I94" s="106"/>
     </row>
     <row r="95" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B95" s="84"/>
-      <c r="C95" s="85"/>
-      <c r="D95" s="85"/>
-      <c r="E95" s="85"/>
-      <c r="F95" s="85"/>
-      <c r="G95" s="85"/>
-      <c r="H95" s="85"/>
-      <c r="I95" s="86"/>
+      <c r="B95" s="107"/>
+      <c r="C95" s="108"/>
+      <c r="D95" s="108"/>
+      <c r="E95" s="108"/>
+      <c r="F95" s="108"/>
+      <c r="G95" s="108"/>
+      <c r="H95" s="108"/>
+      <c r="I95" s="109"/>
     </row>
   </sheetData>
   <mergeCells count="75">
+    <mergeCell ref="J34:M34"/>
+    <mergeCell ref="B52:I61"/>
+    <mergeCell ref="J35:M35"/>
+    <mergeCell ref="J37:M37"/>
+    <mergeCell ref="J38:M38"/>
+    <mergeCell ref="J39:M39"/>
+    <mergeCell ref="B51:I51"/>
+    <mergeCell ref="H43:H44"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="C47:E48"/>
+    <mergeCell ref="G45:G46"/>
+    <mergeCell ref="H45:H46"/>
+    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="G47:G48"/>
+    <mergeCell ref="H47:H48"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B74:I74"/>
+    <mergeCell ref="B86:I95"/>
+    <mergeCell ref="B62:D62"/>
+    <mergeCell ref="E62:I62"/>
+    <mergeCell ref="B64:I64"/>
+    <mergeCell ref="B65:I73"/>
+    <mergeCell ref="B75:I82"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="C45:E46"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="C43:E44"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="G43:G44"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="B4:I4"/>
+    <mergeCell ref="C6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="J93:K93"/>
     <mergeCell ref="B24:E24"/>
     <mergeCell ref="F24:H24"/>
@@ -3676,65 +3735,6 @@
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B3:I3"/>
-    <mergeCell ref="B4:I4"/>
-    <mergeCell ref="C6:I6"/>
-    <mergeCell ref="B5:I5"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="G43:G44"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="C45:E46"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="C43:E44"/>
-    <mergeCell ref="F43:F44"/>
-    <mergeCell ref="B74:I74"/>
-    <mergeCell ref="B86:I95"/>
-    <mergeCell ref="B62:D62"/>
-    <mergeCell ref="E62:I62"/>
-    <mergeCell ref="B64:I64"/>
-    <mergeCell ref="B65:I73"/>
-    <mergeCell ref="B75:I82"/>
-    <mergeCell ref="J34:M34"/>
-    <mergeCell ref="B52:I61"/>
-    <mergeCell ref="J35:M35"/>
-    <mergeCell ref="J37:M37"/>
-    <mergeCell ref="J38:M38"/>
-    <mergeCell ref="J39:M39"/>
-    <mergeCell ref="B51:I51"/>
-    <mergeCell ref="H43:H44"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="C47:E48"/>
-    <mergeCell ref="G45:G46"/>
-    <mergeCell ref="H45:H46"/>
-    <mergeCell ref="F47:F48"/>
-    <mergeCell ref="G47:G48"/>
-    <mergeCell ref="H47:H48"/>
-    <mergeCell ref="B39:C39"/>
   </mergeCells>
   <conditionalFormatting sqref="H27:H32 H36">
     <cfRule type="colorScale" priority="2">
@@ -3771,8 +3771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView showGridLines="0" topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3789,7 +3789,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="126" t="s">
+      <c r="A1" s="127" t="s">
         <v>39</v>
       </c>
       <c r="B1" s="29" t="s">
@@ -3798,23 +3798,23 @@
       <c r="C1" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="127" t="s">
+      <c r="D1" s="128" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="127" t="s">
+      <c r="E1" s="128" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="127" t="s">
+      <c r="F1" s="128" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="126"/>
+      <c r="A2" s="127"/>
       <c r="B2" s="30"/>
       <c r="C2" s="30"/>
-      <c r="D2" s="127"/>
-      <c r="E2" s="127"/>
-      <c r="F2" s="127"/>
+      <c r="D2" s="128"/>
+      <c r="E2" s="128"/>
+      <c r="F2" s="128"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="39" t="s">
@@ -3826,7 +3826,7 @@
       <c r="E3" s="40"/>
       <c r="F3" s="40">
         <f>SUM(D4:D7)</f>
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -3845,7 +3845,7 @@
         <v>98</v>
       </c>
       <c r="D5" s="35">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E5" s="35">
         <v>3</v>
@@ -3873,10 +3873,10 @@
         <f>SUM(D9:D14)</f>
         <v>16</v>
       </c>
-      <c r="G8" s="128" t="s">
+      <c r="G8" s="129" t="s">
         <v>47</v>
       </c>
-      <c r="H8" s="128"/>
+      <c r="H8" s="129"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="31" t="s">
@@ -3888,8 +3888,8 @@
       <c r="E9" s="35">
         <v>3</v>
       </c>
-      <c r="G9" s="128"/>
-      <c r="H9" s="128"/>
+      <c r="G9" s="129"/>
+      <c r="H9" s="129"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
@@ -3901,8 +3901,8 @@
       <c r="E10" s="35">
         <v>3</v>
       </c>
-      <c r="G10" s="128"/>
-      <c r="H10" s="128"/>
+      <c r="G10" s="129"/>
+      <c r="H10" s="129"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
@@ -3914,8 +3914,8 @@
       <c r="E11" s="35">
         <v>3</v>
       </c>
-      <c r="G11" s="128"/>
-      <c r="H11" s="128"/>
+      <c r="G11" s="129"/>
+      <c r="H11" s="129"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="31" t="s">
@@ -3927,8 +3927,8 @@
       <c r="E12" s="35">
         <v>3</v>
       </c>
-      <c r="G12" s="128"/>
-      <c r="H12" s="128"/>
+      <c r="G12" s="129"/>
+      <c r="H12" s="129"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -3940,8 +3940,8 @@
       <c r="E13" s="35">
         <v>3</v>
       </c>
-      <c r="G13" s="128"/>
-      <c r="H13" s="128"/>
+      <c r="G13" s="129"/>
+      <c r="H13" s="129"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="31" t="s">
@@ -3953,8 +3953,8 @@
       <c r="E14" s="35">
         <v>3</v>
       </c>
-      <c r="G14" s="128"/>
-      <c r="H14" s="128"/>
+      <c r="G14" s="129"/>
+      <c r="H14" s="129"/>
     </row>
     <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="39" t="s">
@@ -3968,8 +3968,8 @@
         <f>SUM(D16:D20)</f>
         <v>24</v>
       </c>
-      <c r="G15" s="128"/>
-      <c r="H15" s="128"/>
+      <c r="G15" s="129"/>
+      <c r="H15" s="129"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="31" t="s">
@@ -3981,8 +3981,8 @@
       <c r="E16" s="36">
         <v>3</v>
       </c>
-      <c r="G16" s="128"/>
-      <c r="H16" s="128"/>
+      <c r="G16" s="129"/>
+      <c r="H16" s="129"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="53" t="s">
@@ -3994,8 +3994,8 @@
       <c r="E17" s="36">
         <v>3</v>
       </c>
-      <c r="G17" s="128"/>
-      <c r="H17" s="128"/>
+      <c r="G17" s="129"/>
+      <c r="H17" s="129"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="53" t="s">
@@ -4007,8 +4007,8 @@
       <c r="E18" s="36">
         <v>3</v>
       </c>
-      <c r="G18" s="128"/>
-      <c r="H18" s="128"/>
+      <c r="G18" s="129"/>
+      <c r="H18" s="129"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="53" t="s">
@@ -4020,8 +4020,8 @@
       <c r="E19" s="36">
         <v>3</v>
       </c>
-      <c r="G19" s="128"/>
-      <c r="H19" s="128"/>
+      <c r="G19" s="129"/>
+      <c r="H19" s="129"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
@@ -4033,8 +4033,8 @@
       <c r="E20" s="36">
         <v>3</v>
       </c>
-      <c r="G20" s="128"/>
-      <c r="H20" s="128"/>
+      <c r="G20" s="129"/>
+      <c r="H20" s="129"/>
     </row>
     <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="39" t="s">
@@ -4048,8 +4048,8 @@
         <f>SUM(D22:D26)</f>
         <v>29</v>
       </c>
-      <c r="G21" s="128"/>
-      <c r="H21" s="128"/>
+      <c r="G21" s="129"/>
+      <c r="H21" s="129"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="31" t="s">
@@ -4273,7 +4273,7 @@
       <c r="C38" s="38"/>
       <c r="D38" s="38">
         <f>SUM(F3:F32)</f>
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E38" s="38"/>
       <c r="F38" s="32"/>
@@ -4287,7 +4287,7 @@
       </c>
       <c r="D40" s="41">
         <f>D38*F40</f>
-        <v>40.799999999999997</v>
+        <v>39.9</v>
       </c>
       <c r="E40" s="33"/>
       <c r="F40" s="46">
@@ -4304,7 +4304,7 @@
       <c r="C41" s="34"/>
       <c r="D41" s="42">
         <f>SUM(D38:D40)</f>
-        <v>176.8</v>
+        <v>172.9</v>
       </c>
       <c r="E41" s="43"/>
       <c r="F41" s="44"/>
@@ -4316,46 +4316,48 @@
       <c r="A44" s="50" t="s">
         <v>59</v>
       </c>
-      <c r="D44" s="129" t="s">
+      <c r="D44" s="126" t="s">
         <v>60</v>
       </c>
-      <c r="E44" s="129"/>
+      <c r="E44" s="126"/>
       <c r="F44" s="49">
         <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D45" s="129" t="s">
+      <c r="D45" s="126" t="s">
         <v>61</v>
       </c>
-      <c r="E45" s="129"/>
+      <c r="E45" s="126"/>
       <c r="F45" s="48">
         <v>9</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D46" s="129" t="s">
+      <c r="D46" s="126" t="s">
         <v>62</v>
       </c>
-      <c r="E46" s="129"/>
+      <c r="E46" s="126"/>
       <c r="F46" s="48">
         <f>F45*F44</f>
         <v>27</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D47" s="129" t="s">
+      <c r="D47" s="126" t="s">
         <v>63</v>
       </c>
-      <c r="E47" s="129"/>
+      <c r="E47" s="126"/>
       <c r="F47" s="47">
         <f>D38/F45</f>
-        <v>15.111111111111111</v>
+        <v>14.777777777777779</v>
       </c>
       <c r="G47" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G8:H21"/>
     <mergeCell ref="D44:E44"/>
     <mergeCell ref="D45:E45"/>
     <mergeCell ref="D47:E47"/>
@@ -4363,8 +4365,6 @@
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G8:H21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>